<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@cb62d23ad5f9765f54dca4e44d2d5bc467512cfa 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
+++ b/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
@@ -25,12 +25,12 @@
     <t>status</t>
   </si>
   <si>
+    <t>codeforiati:group-code</t>
+  </si>
+  <si>
     <t>codeforiati:group-name</t>
   </si>
   <si>
-    <t>codeforiati:group-code</t>
-  </si>
-  <si>
     <t>BE-BCE_KBO-0264814354</t>
   </si>
   <si>
@@ -40,12 +40,12 @@
     <t>active</t>
   </si>
   <si>
+    <t>BE</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
     <t>XM-DAC-2-10</t>
   </si>
   <si>
@@ -58,12 +58,12 @@
     <t>Canada - Global Affairs Canada | Affaires mondiales Canada</t>
   </si>
   <si>
+    <t>CA</t>
+  </si>
+  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
     <t>CA-4</t>
   </si>
   <si>
@@ -76,12 +76,12 @@
     <t>Germany - Ministry for Economic Cooperation and Development</t>
   </si>
   <si>
+    <t>DE</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>DE</t>
-  </si>
-  <si>
     <t>XI-IATI-IKI</t>
   </si>
   <si>
@@ -106,12 +106,12 @@
     <t>European Commission - Humanitarian Aid &amp; Civil Protection</t>
   </si>
   <si>
+    <t>EC</t>
+  </si>
+  <si>
     <t>European Commission</t>
   </si>
   <si>
-    <t>EC</t>
-  </si>
-  <si>
     <t>XI-IATI-EC_INTPA</t>
   </si>
   <si>
@@ -130,12 +130,12 @@
     <t>Spain - Ministry of Foreign Affairs and Cooperation</t>
   </si>
   <si>
+    <t>ES</t>
+  </si>
+  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>ES</t>
-  </si>
-  <si>
     <t>XM-DAC-50-21</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>Agence Française de Développement</t>
   </si>
   <si>
+    <t>FR</t>
+  </si>
+  <si>
     <t>France</t>
   </si>
   <si>
-    <t>FR</t>
-  </si>
-  <si>
     <t>FR-6</t>
   </si>
   <si>
@@ -166,12 +166,12 @@
     <t>UK - Department for Work and Pensions</t>
   </si>
   <si>
+    <t>GB</t>
+  </si>
+  <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>GB</t>
-  </si>
-  <si>
     <t>GB-GOV-9</t>
   </si>
   <si>
@@ -277,12 +277,12 @@
     <t>Ministry of Foreign Affairs of Japan</t>
   </si>
   <si>
+    <t>JP</t>
+  </si>
+  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>JP</t>
-  </si>
-  <si>
     <t>XM-DAC-701-8</t>
   </si>
   <si>
@@ -295,12 +295,12 @@
     <t>Kadaster International</t>
   </si>
   <si>
+    <t>NL</t>
+  </si>
+  <si>
     <t>Netherlands</t>
   </si>
   <si>
-    <t>NL</t>
-  </si>
-  <si>
     <t>NL-KVK-27367015</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>UN-Habitat</t>
   </si>
   <si>
+    <t>UN</t>
+  </si>
+  <si>
     <t>United Nations</t>
   </si>
   <si>
-    <t>UN</t>
-  </si>
-  <si>
     <t>41AAA</t>
   </si>
   <si>
@@ -499,12 +499,12 @@
     <t>Millennium Challenge Corporation</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>United States</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>US-18</t>
   </si>
   <si>
@@ -637,10 +637,10 @@
     <t>The World Bank</t>
   </si>
   <si>
+    <t>WB</t>
+  </si>
+  <si>
     <t>World Bank Group</t>
-  </si>
-  <si>
-    <t>WB</t>
   </si>
   <si>
     <t>XI-IATI-WBTF</t>
@@ -2525,7 +2525,7 @@
         <v>204</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@91fa57d84c5da6f03203a179a8555ea2c1c6a4f1 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
+++ b/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
@@ -25,12 +25,12 @@
     <t>status</t>
   </si>
   <si>
+    <t>codeforiati:group-name</t>
+  </si>
+  <si>
     <t>codeforiati:group-code</t>
   </si>
   <si>
-    <t>codeforiati:group-name</t>
-  </si>
-  <si>
     <t>BE-BCE_KBO-0264814354</t>
   </si>
   <si>
@@ -40,12 +40,12 @@
     <t>active</t>
   </si>
   <si>
+    <t>Belgium</t>
+  </si>
+  <si>
     <t>BE</t>
   </si>
   <si>
-    <t>Belgium</t>
-  </si>
-  <si>
     <t>XM-DAC-2-10</t>
   </si>
   <si>
@@ -58,12 +58,12 @@
     <t>Canada - Global Affairs Canada | Affaires mondiales Canada</t>
   </si>
   <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>CA</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>CA-4</t>
   </si>
   <si>
@@ -76,12 +76,12 @@
     <t>Germany - Ministry for Economic Cooperation and Development</t>
   </si>
   <si>
+    <t>Germany</t>
+  </si>
+  <si>
     <t>DE</t>
   </si>
   <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>XI-IATI-IKI</t>
   </si>
   <si>
@@ -106,12 +106,12 @@
     <t>European Commission - Humanitarian Aid &amp; Civil Protection</t>
   </si>
   <si>
+    <t>European Commission</t>
+  </si>
+  <si>
     <t>EC</t>
   </si>
   <si>
-    <t>European Commission</t>
-  </si>
-  <si>
     <t>XI-IATI-EC_INTPA</t>
   </si>
   <si>
@@ -130,12 +130,12 @@
     <t>Spain - Ministry of Foreign Affairs and Cooperation</t>
   </si>
   <si>
+    <t>Spain</t>
+  </si>
+  <si>
     <t>ES</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
     <t>XM-DAC-50-21</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>Agence Française de Développement</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
     <t>FR</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
     <t>FR-6</t>
   </si>
   <si>
@@ -166,12 +166,12 @@
     <t>UK - Department for Work and Pensions</t>
   </si>
   <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
     <t>GB</t>
   </si>
   <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>GB-GOV-9</t>
   </si>
   <si>
@@ -277,12 +277,12 @@
     <t>Ministry of Foreign Affairs of Japan</t>
   </si>
   <si>
+    <t>Japan</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
-    <t>Japan</t>
-  </si>
-  <si>
     <t>XM-DAC-701-8</t>
   </si>
   <si>
@@ -295,12 +295,12 @@
     <t>Kadaster International</t>
   </si>
   <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
     <t>NL</t>
   </si>
   <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
     <t>NL-KVK-27367015</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>UN-Habitat</t>
   </si>
   <si>
+    <t>United Nations</t>
+  </si>
+  <si>
     <t>UN</t>
   </si>
   <si>
-    <t>United Nations</t>
-  </si>
-  <si>
     <t>41AAA</t>
   </si>
   <si>
@@ -499,12 +499,12 @@
     <t>Millennium Challenge Corporation</t>
   </si>
   <si>
+    <t>United States</t>
+  </si>
+  <si>
     <t>US</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>US-18</t>
   </si>
   <si>
@@ -637,10 +637,10 @@
     <t>The World Bank</t>
   </si>
   <si>
+    <t>World Bank Group</t>
+  </si>
+  <si>
     <t>WB</t>
-  </si>
-  <si>
-    <t>World Bank Group</t>
   </si>
   <si>
     <t>XI-IATI-WBTF</t>
@@ -2525,7 +2525,7 @@
         <v>204</v>
       </c>
       <c r="B91" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C91" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@97b2f69cbdbde00596ae791ddb18422979032350 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
+++ b/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
@@ -25,12 +25,12 @@
     <t>status</t>
   </si>
   <si>
+    <t>codeforiati:group-code</t>
+  </si>
+  <si>
     <t>codeforiati:group-name</t>
   </si>
   <si>
-    <t>codeforiati:group-code</t>
-  </si>
-  <si>
     <t>BE-BCE_KBO-0264814354</t>
   </si>
   <si>
@@ -40,12 +40,12 @@
     <t>active</t>
   </si>
   <si>
+    <t>BE</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
     <t>XM-DAC-2-10</t>
   </si>
   <si>
@@ -58,12 +58,12 @@
     <t>Canada - Global Affairs Canada | Affaires mondiales Canada</t>
   </si>
   <si>
+    <t>CA</t>
+  </si>
+  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
     <t>CA-4</t>
   </si>
   <si>
@@ -76,12 +76,12 @@
     <t>Germany - Ministry for Economic Cooperation and Development</t>
   </si>
   <si>
+    <t>DE</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>DE</t>
-  </si>
-  <si>
     <t>XI-IATI-IKI</t>
   </si>
   <si>
@@ -106,12 +106,12 @@
     <t>European Commission - Humanitarian Aid &amp; Civil Protection</t>
   </si>
   <si>
+    <t>EC</t>
+  </si>
+  <si>
     <t>European Commission</t>
   </si>
   <si>
-    <t>EC</t>
-  </si>
-  <si>
     <t>XI-IATI-EC_INTPA</t>
   </si>
   <si>
@@ -130,12 +130,12 @@
     <t>Spain - Ministry of Foreign Affairs and Cooperation</t>
   </si>
   <si>
+    <t>ES</t>
+  </si>
+  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>ES</t>
-  </si>
-  <si>
     <t>XM-DAC-50-21</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>Agence Française de Développement</t>
   </si>
   <si>
+    <t>FR</t>
+  </si>
+  <si>
     <t>France</t>
   </si>
   <si>
-    <t>FR</t>
-  </si>
-  <si>
     <t>FR-6</t>
   </si>
   <si>
@@ -166,12 +166,12 @@
     <t>UK - Department for Work and Pensions</t>
   </si>
   <si>
+    <t>GB</t>
+  </si>
+  <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>GB</t>
-  </si>
-  <si>
     <t>GB-GOV-9</t>
   </si>
   <si>
@@ -277,12 +277,12 @@
     <t>Ministry of Foreign Affairs of Japan</t>
   </si>
   <si>
+    <t>JP</t>
+  </si>
+  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>JP</t>
-  </si>
-  <si>
     <t>XM-DAC-701-8</t>
   </si>
   <si>
@@ -295,12 +295,12 @@
     <t>Kadaster International</t>
   </si>
   <si>
+    <t>NL</t>
+  </si>
+  <si>
     <t>Netherlands</t>
   </si>
   <si>
-    <t>NL</t>
-  </si>
-  <si>
     <t>NL-KVK-27367015</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>UN-Habitat</t>
   </si>
   <si>
+    <t>UN</t>
+  </si>
+  <si>
     <t>United Nations</t>
   </si>
   <si>
-    <t>UN</t>
-  </si>
-  <si>
     <t>41AAA</t>
   </si>
   <si>
@@ -499,12 +499,12 @@
     <t>Millennium Challenge Corporation</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>United States</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>US-18</t>
   </si>
   <si>
@@ -637,10 +637,10 @@
     <t>The World Bank</t>
   </si>
   <si>
+    <t>WB</t>
+  </si>
+  <si>
     <t>World Bank Group</t>
-  </si>
-  <si>
-    <t>WB</t>
   </si>
   <si>
     <t>XI-IATI-WBTF</t>
@@ -2525,7 +2525,7 @@
         <v>204</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@014ad6fcea0684c5d63b9e87249db0675c32a414 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
+++ b/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
@@ -25,12 +25,12 @@
     <t>status</t>
   </si>
   <si>
+    <t>codeforiati:group-name</t>
+  </si>
+  <si>
     <t>codeforiati:group-code</t>
   </si>
   <si>
-    <t>codeforiati:group-name</t>
-  </si>
-  <si>
     <t>BE-BCE_KBO-0264814354</t>
   </si>
   <si>
@@ -40,12 +40,12 @@
     <t>active</t>
   </si>
   <si>
+    <t>Belgium</t>
+  </si>
+  <si>
     <t>BE</t>
   </si>
   <si>
-    <t>Belgium</t>
-  </si>
-  <si>
     <t>XM-DAC-2-10</t>
   </si>
   <si>
@@ -58,12 +58,12 @@
     <t>Canada - Global Affairs Canada | Affaires mondiales Canada</t>
   </si>
   <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>CA</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>CA-4</t>
   </si>
   <si>
@@ -76,12 +76,12 @@
     <t>Germany - Ministry for Economic Cooperation and Development</t>
   </si>
   <si>
+    <t>Germany</t>
+  </si>
+  <si>
     <t>DE</t>
   </si>
   <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>XI-IATI-IKI</t>
   </si>
   <si>
@@ -106,12 +106,12 @@
     <t>European Commission - Humanitarian Aid &amp; Civil Protection</t>
   </si>
   <si>
+    <t>European Commission</t>
+  </si>
+  <si>
     <t>EC</t>
   </si>
   <si>
-    <t>European Commission</t>
-  </si>
-  <si>
     <t>XI-IATI-EC_INTPA</t>
   </si>
   <si>
@@ -130,12 +130,12 @@
     <t>Spain - Ministry of Foreign Affairs and Cooperation</t>
   </si>
   <si>
+    <t>Spain</t>
+  </si>
+  <si>
     <t>ES</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
     <t>XM-DAC-50-21</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>Agence Française de Développement</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
     <t>FR</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
     <t>FR-6</t>
   </si>
   <si>
@@ -166,12 +166,12 @@
     <t>UK - Department for Work and Pensions</t>
   </si>
   <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
     <t>GB</t>
   </si>
   <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>GB-GOV-9</t>
   </si>
   <si>
@@ -277,12 +277,12 @@
     <t>Ministry of Foreign Affairs of Japan</t>
   </si>
   <si>
+    <t>Japan</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
-    <t>Japan</t>
-  </si>
-  <si>
     <t>XM-DAC-701-8</t>
   </si>
   <si>
@@ -295,12 +295,12 @@
     <t>Kadaster International</t>
   </si>
   <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
     <t>NL</t>
   </si>
   <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
     <t>NL-KVK-27367015</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>UN-Habitat</t>
   </si>
   <si>
+    <t>United Nations</t>
+  </si>
+  <si>
     <t>UN</t>
   </si>
   <si>
-    <t>United Nations</t>
-  </si>
-  <si>
     <t>41AAA</t>
   </si>
   <si>
@@ -499,12 +499,12 @@
     <t>Millennium Challenge Corporation</t>
   </si>
   <si>
+    <t>United States</t>
+  </si>
+  <si>
     <t>US</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>US-18</t>
   </si>
   <si>
@@ -637,10 +637,10 @@
     <t>The World Bank</t>
   </si>
   <si>
+    <t>World Bank Group</t>
+  </si>
+  <si>
     <t>WB</t>
-  </si>
-  <si>
-    <t>World Bank Group</t>
   </si>
   <si>
     <t>XI-IATI-WBTF</t>
@@ -2525,7 +2525,7 @@
         <v>204</v>
       </c>
       <c r="B91" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C91" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@620b1f1f0a3c7901cc6073ea6bc3f915ed264bf3 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
+++ b/api/1/clv2/xlsx/en/ReportingOrganisationGroup.xlsx
@@ -25,12 +25,12 @@
     <t>status</t>
   </si>
   <si>
+    <t>codeforiati:group-code</t>
+  </si>
+  <si>
     <t>codeforiati:group-name</t>
   </si>
   <si>
-    <t>codeforiati:group-code</t>
-  </si>
-  <si>
     <t>BE-BCE_KBO-0264814354</t>
   </si>
   <si>
@@ -40,12 +40,12 @@
     <t>active</t>
   </si>
   <si>
+    <t>BE</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
     <t>XM-DAC-2-10</t>
   </si>
   <si>
@@ -58,12 +58,12 @@
     <t>Canada - Global Affairs Canada | Affaires mondiales Canada</t>
   </si>
   <si>
+    <t>CA</t>
+  </si>
+  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
     <t>CA-4</t>
   </si>
   <si>
@@ -76,12 +76,12 @@
     <t>Germany - Ministry for Economic Cooperation and Development</t>
   </si>
   <si>
+    <t>DE</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>DE</t>
-  </si>
-  <si>
     <t>XI-IATI-IKI</t>
   </si>
   <si>
@@ -106,12 +106,12 @@
     <t>European Commission - Humanitarian Aid &amp; Civil Protection</t>
   </si>
   <si>
+    <t>EC</t>
+  </si>
+  <si>
     <t>European Commission</t>
   </si>
   <si>
-    <t>EC</t>
-  </si>
-  <si>
     <t>XI-IATI-EC_INTPA</t>
   </si>
   <si>
@@ -130,12 +130,12 @@
     <t>Spain - Ministry of Foreign Affairs and Cooperation</t>
   </si>
   <si>
+    <t>ES</t>
+  </si>
+  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>ES</t>
-  </si>
-  <si>
     <t>XM-DAC-50-21</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>Agence Française de Développement</t>
   </si>
   <si>
+    <t>FR</t>
+  </si>
+  <si>
     <t>France</t>
   </si>
   <si>
-    <t>FR</t>
-  </si>
-  <si>
     <t>FR-6</t>
   </si>
   <si>
@@ -166,12 +166,12 @@
     <t>UK - Department for Work and Pensions</t>
   </si>
   <si>
+    <t>GB</t>
+  </si>
+  <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>GB</t>
-  </si>
-  <si>
     <t>GB-GOV-9</t>
   </si>
   <si>
@@ -277,12 +277,12 @@
     <t>Ministry of Foreign Affairs of Japan</t>
   </si>
   <si>
+    <t>JP</t>
+  </si>
+  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>JP</t>
-  </si>
-  <si>
     <t>XM-DAC-701-8</t>
   </si>
   <si>
@@ -295,12 +295,12 @@
     <t>Kadaster International</t>
   </si>
   <si>
+    <t>NL</t>
+  </si>
+  <si>
     <t>Netherlands</t>
   </si>
   <si>
-    <t>NL</t>
-  </si>
-  <si>
     <t>NL-KVK-27367015</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>UN-Habitat</t>
   </si>
   <si>
+    <t>UN</t>
+  </si>
+  <si>
     <t>United Nations</t>
   </si>
   <si>
-    <t>UN</t>
-  </si>
-  <si>
     <t>41AAA</t>
   </si>
   <si>
@@ -499,12 +499,12 @@
     <t>Millennium Challenge Corporation</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>United States</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>US-18</t>
   </si>
   <si>
@@ -637,10 +637,10 @@
     <t>The World Bank</t>
   </si>
   <si>
+    <t>WB</t>
+  </si>
+  <si>
     <t>World Bank Group</t>
-  </si>
-  <si>
-    <t>WB</t>
   </si>
   <si>
     <t>XI-IATI-WBTF</t>
@@ -2525,7 +2525,7 @@
         <v>204</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
         <v>53</v>

</xml_diff>